<commit_message>
completed bank account test plans
</commit_message>
<xml_diff>
--- a/tests/A01_pixell_test_plan_bank_account.xlsx
+++ b/tests/A01_pixell_test_plan_bank_account.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
   <si>
     <t>#VALUE!</t>
   </si>
@@ -58,64 +58,160 @@
     <t>Attributes are set to input values.</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>40075,                                                       2828,                                                             640.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object created with correct values                                     </t>
+  </si>
+  <si>
     <t>Balance attribute set to 0 when non-numeric balance argument.</t>
   </si>
   <si>
+    <t>40075,                                                                 2828,                                                        "beautiful"</t>
+  </si>
+  <si>
+    <t>balance = 0.0</t>
+  </si>
+  <si>
     <t>ValueError when non-numeric account number</t>
   </si>
   <si>
+    <t>"bad", 2828, 640.00</t>
+  </si>
+  <si>
+    <t>Raises ValueError</t>
+  </si>
+  <si>
     <t>ValueError when non-numeric client number</t>
   </si>
   <si>
+    <t>40075, "bad", 640.00</t>
+  </si>
+  <si>
     <t>account_number (getter)</t>
   </si>
   <si>
     <t>returns account number attribute</t>
   </si>
   <si>
+    <t>Account exists</t>
+  </si>
+  <si>
+    <t>Returns 40075</t>
+  </si>
+  <si>
     <t>client_number (getter)</t>
   </si>
   <si>
     <t>returns client number attribute</t>
   </si>
   <si>
+    <t>Returns 2828</t>
+  </si>
+  <si>
     <t>balance (getter)</t>
   </si>
   <si>
     <t>returns balance attribute</t>
   </si>
   <si>
+    <t>Returns 640.00</t>
+  </si>
+  <si>
     <t>update_balance</t>
   </si>
   <si>
     <t>correctly updates balance attribute when positive amount is received.</t>
   </si>
   <si>
+    <t>Account with=140.00</t>
+  </si>
+  <si>
+    <t>amount=50.00</t>
+  </si>
+  <si>
+    <t>balance=190</t>
+  </si>
+  <si>
     <t>correctly updates balance attribute when negative amount is received.</t>
   </si>
   <si>
+    <t>Account with=90.00</t>
+  </si>
+  <si>
+    <t>amount=-40</t>
+  </si>
+  <si>
+    <t>balance=50.00</t>
+  </si>
+  <si>
     <t>Balance attribute value remains unchanged when amount is non-numeric</t>
   </si>
   <si>
+    <t>Account with=200.00</t>
+  </si>
+  <si>
+    <t>amount="beautiful"</t>
+  </si>
+  <si>
+    <t>balance=200.00</t>
+  </si>
+  <si>
     <t>deposit</t>
   </si>
   <si>
     <t>BankAccount object's balance is updated correctly when a valid amount is provided.</t>
   </si>
   <si>
+    <t>balance=250.00</t>
+  </si>
+  <si>
     <t>ValueError when negative amount is provided.</t>
   </si>
   <si>
+    <t>Account with=100.00</t>
+  </si>
+  <si>
+    <t>amount=-50</t>
+  </si>
+  <si>
     <t>withdraw</t>
   </si>
   <si>
+    <t>Account with= 250.00</t>
+  </si>
+  <si>
+    <t>amount=50</t>
+  </si>
+  <si>
+    <t>Account with &gt;0</t>
+  </si>
+  <si>
+    <t>amount =-20</t>
+  </si>
+  <si>
     <t>ValueError when amount exceeds balance.</t>
   </si>
   <si>
+    <t>Account with=50.00</t>
+  </si>
+  <si>
+    <t>amount=100.00</t>
+  </si>
+  <si>
     <t>__str__</t>
   </si>
   <si>
     <t>returns string in expected format.</t>
+  </si>
+  <si>
+    <t>Account with=640.00</t>
+  </si>
+  <si>
+    <t>"Account Number:                                 40075\nClient Number:                               2828\nBalance:                                       $640.00</t>
   </si>
   <si>
     <t>Add more rows as necessary</t>
@@ -956,7 +1052,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="16">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="49.5" customFormat="1" s="16">
       <c r="A7" s="17"/>
       <c r="B7" s="18">
         <v>1</v>
@@ -967,11 +1063,17 @@
       <c r="D7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="31.5" customFormat="1" s="16">
+      <c r="E7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="52.5" customFormat="1" s="16">
       <c r="A8" s="17"/>
       <c r="B8" s="21">
         <v>2</v>
@@ -980,11 +1082,17 @@
         <v>12</v>
       </c>
       <c r="D8" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="23"/>
+      <c r="F8" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="31.149999999999995">
       <c r="A9" s="1"/>
@@ -995,11 +1103,17 @@
         <v>12</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
+        <v>20</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
       <c r="A10" s="17"/>
@@ -1010,11 +1124,17 @@
         <v>12</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
+        <v>23</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
       <c r="A11" s="17"/>
@@ -1022,14 +1142,20 @@
         <v>5</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
+        <v>26</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
       <c r="A12" s="17"/>
@@ -1037,14 +1163,20 @@
         <v>6</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
+        <v>30</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
       <c r="A13" s="17"/>
@@ -1052,14 +1184,20 @@
         <v>7</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
+        <v>33</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="31.149999999999995">
       <c r="A14" s="1"/>
@@ -1067,14 +1205,20 @@
         <v>8</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
+        <v>36</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="47.25" customFormat="1" s="16">
       <c r="A15" s="17"/>
@@ -1082,29 +1226,41 @@
         <v>9</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
+        <v>40</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="63.75" customFormat="1" s="16">
       <c r="A16" s="17"/>
       <c r="B16" s="18">
         <v>10</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
+        <v>44</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="51" customFormat="1" s="16">
       <c r="A17" s="17"/>
@@ -1112,14 +1268,20 @@
         <v>11</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
+        <v>49</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
       <c r="A18" s="17"/>
@@ -1127,29 +1289,41 @@
         <v>12</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="31.149999999999995">
+        <v>51</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="60.75">
       <c r="A19" s="1"/>
       <c r="B19" s="24">
         <v>13</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
+        <v>49</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
       <c r="A20" s="17"/>
@@ -1157,14 +1331,20 @@
         <v>14</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
+        <v>51</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
       <c r="A21" s="17"/>
@@ -1172,29 +1352,41 @@
         <v>15</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
+        <v>59</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="66.75" customFormat="1" s="16">
       <c r="A22" s="17"/>
       <c r="B22" s="18">
         <v>16</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
+        <v>63</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
       <c r="A23" s="17"/>
@@ -1373,7 +1565,7 @@
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="1"/>
       <c r="B39" s="27" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="C39" s="28"/>
       <c r="D39" s="28"/>

</xml_diff>